<commit_message>
Small correction to template and test.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Container_creation_vtest.xlsx
+++ b/backend/fms_core/static/submission_templates/Container_creation_vtest.xlsx
@@ -440,7 +440,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="22.33"/>
@@ -4796,7 +4796,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="9.33"/>

</xml_diff>

<commit_message>
Small correction to template and test. (#155)
* Small correction to template and test.

* Small correction to test.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Container_creation_vtest.xlsx
+++ b/backend/fms_core/static/submission_templates/Container_creation_vtest.xlsx
@@ -440,7 +440,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="22.33"/>
@@ -4796,7 +4796,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="9.33"/>

</xml_diff>

<commit_message>
small changes to propagate adjustments to v3.4.1 into master
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Container_creation_vtest.xlsx
+++ b/backend/fms_core/static/submission_templates/Container_creation_vtest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t xml:space="preserve">Container Creation Template</t>
   </si>
@@ -74,6 +74,9 @@
     <t xml:space="preserve">Freezer rack 2x4</t>
   </si>
   <si>
+    <t xml:space="preserve">Freezer rack 3x4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Freezer rack 4x4</t>
   </si>
   <si>
@@ -86,7 +89,16 @@
     <t xml:space="preserve">Freezer rack 7x4</t>
   </si>
   <si>
+    <t xml:space="preserve">Freezer rack 10x5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Freezer rack 8x6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freezer rack 11x6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freezer rack 11x7</t>
   </si>
   <si>
     <t xml:space="preserve">Freezer 3 shelves</t>
@@ -452,9 +464,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="22.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.33"/>
@@ -4783,7 +4795,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A8:A107" type="list">
-      <formula1>Index!$A$2:$A$20</formula1>
+      <formula1>Index!$A$2:$A$24</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -4802,13 +4814,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A1009"/>
+  <dimension ref="A1:A1013"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="9.33"/>
@@ -4864,12 +4876,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
         <v>18</v>
       </c>
@@ -4879,7 +4891,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
@@ -4889,35 +4901,51 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5894,6 +5922,10 @@
     <row r="1007" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1008" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1009" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1010" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1011" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1012" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1013" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>